<commit_message>
changes to analysis files
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="97">
   <si>
     <t>parameter_name</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>prob_still_birth_obstructed_labour</t>
+  </si>
+  <si>
+    <t>baseline_prev_cs</t>
   </si>
 </sst>
 </file>
@@ -1128,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1158,267 +1161,273 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B3">
-        <v>0.03</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="B4">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>0.03</v>
+      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>1.47</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>1.57</v>
+        <v>1.47</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>1.3</v>
+        <v>1.57</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>0.09</v>
+        <v>1.3</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B9">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="C9">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B10">
-        <v>1.73</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>2.63</v>
+        <v>1.73</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>1.95</v>
+        <v>2.63</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>0.11</v>
+        <v>1.95</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>2.0699999999999998</v>
+        <v>0.11</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>3.2000000000000001E-2</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>0.01</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>1.2E-2</v>
+        <v>0.01</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>5.0000000000000001E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>3.4</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>1E-3</v>
+        <v>3.4</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>7.57</v>
+        <v>1E-3</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>2.02</v>
+        <v>7.57</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>23.65</v>
+        <v>2.02</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>1.4</v>
+        <v>23.65</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>1.95</v>
+        <v>1.4</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>2.04</v>
+        <v>1.95</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>0.5</v>
+        <v>2.04</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>1.72</v>
+        <v>0.5</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>9.1</v>
+        <v>1.72</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="B30">
-        <v>4.0000000000000001E-3</v>
+        <v>9.1</v>
       </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="B31">
-        <v>0.02</v>
-      </c>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>0.02</v>
@@ -1426,199 +1435,199 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>0.184</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>0.33</v>
+        <v>0.184</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="B35">
-        <v>0.34499999999999997</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="B36">
-        <v>0.38</v>
+        <v>0.34499999999999997</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="B37">
-        <v>0.9</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38">
-        <v>0.38</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39">
-        <v>0.9</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40">
-        <v>0.25</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41">
-        <v>0.9</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42">
-        <v>0.93</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B43">
-        <v>0.98</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B44">
-        <v>0.03</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45">
-        <v>0.9</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46">
-        <v>0.01</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48">
-        <v>5</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49">
-        <v>0.05</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B50">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B51">
-        <v>0.184</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52">
-        <v>0.33</v>
+        <v>0.184</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53">
-        <v>0.15</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B54">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55">
-        <v>0.76100000000000001</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56">
-        <v>0.7</v>
+        <v>0.76100000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57">
         <v>0.7</v>
@@ -1626,7 +1635,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="B58">
         <v>0.7</v>
@@ -1634,103 +1643,103 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B59">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="B60">
-        <v>0.34</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B61">
-        <v>0.5</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="B62">
-        <v>0.56999999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B63">
-        <v>0.41</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B64">
-        <v>0.8</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B67">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B68">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B69">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B70">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="B71">
         <v>0.8</v>
@@ -1738,31 +1747,31 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="B72">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B73">
-        <v>0.75</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B74">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B75">
         <v>0.7</v>
@@ -1770,9 +1779,17 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B76">
+      <c r="B77">
         <v>0.7</v>
       </c>
     </row>
@@ -1787,7 +1804,7 @@
   <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Merged in most recent update to master and continued work on edits from draft PR
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -1131,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1142,7 +1142,7 @@
     <col min="1" max="1" width="44.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1159,7 +1159,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>88</v>
       </c>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1204,7 +1204,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1213,21 +1213,24 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
         <v>0.02</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0.09</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -1236,7 +1239,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1245,7 +1248,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1254,7 +1257,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1263,7 +1266,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1272,7 +1275,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1281,7 +1284,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
updates from PR comments
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -1131,15 +1131,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:XFD78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="44.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1795,6 +1796,9 @@
       <c r="B77">
         <v>0.7</v>
       </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new death function, test updates
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="100">
   <si>
     <t>parameter_name</t>
   </si>
@@ -311,6 +311,15 @@
   </si>
   <si>
     <t>baseline_prev_cs</t>
+  </si>
+  <si>
+    <t>prob_still_birth_uterine_rupture</t>
+  </si>
+  <si>
+    <t>prob_still_birth_uterine_rupture_md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correct: </t>
   </si>
 </sst>
 </file>
@@ -1133,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78:XFD78"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,6 +1222,9 @@
         <v>1.3</v>
       </c>
       <c r="D8" s="2"/>
+      <c r="E8" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1519,7 +1531,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="B43">
         <v>0.93</v>
@@ -1527,7 +1539,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="B44">
         <v>0.98</v>

</xml_diff>

<commit_message>
edits to ensure df.dtypes==orig.dtypes. (all tests in pytest now running)
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="101">
   <si>
     <t>parameter_name</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t xml:space="preserve">correct: </t>
+  </si>
+  <si>
+    <t>cfr_pp_pph</t>
   </si>
 </sst>
 </file>
@@ -1142,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M60" sqref="M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1595,7 +1598,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="B51">
         <v>0.1</v>

</xml_diff>

<commit_message>
first bit of work around linear functions in labour code
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -1145,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M60" sqref="M60"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1195,6 +1195,9 @@
         <v>6</v>
       </c>
       <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D5" s="2"/>
@@ -1452,7 +1455,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>71</v>
       </c>
@@ -1476,7 +1479,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -1484,7 +1487,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>95</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -1508,7 +1511,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -1516,7 +1519,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
@@ -1524,7 +1527,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>97</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>98</v>
       </c>
@@ -1548,7 +1551,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -1556,7 +1559,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>42</v>
       </c>
@@ -1564,7 +1567,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
@@ -1572,11 +1575,14 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48">
         <v>0.03</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ongoing abstraction of repeat lines of code
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="103">
   <si>
     <t>parameter_name</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>cfr_pp_pph</t>
+  </si>
+  <si>
+    <t>baseline_prev_labour_states</t>
+  </si>
+  <si>
+    <t>[0.04, 0.12, 0.80, 0.04]</t>
   </si>
 </sst>
 </file>
@@ -815,13 +821,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1143,16 +1152,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="44.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1251,528 +1260,528 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B11">
-        <v>1.73</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>2.63</v>
+        <v>1.73</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>1.95</v>
+        <v>2.63</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>0.11</v>
+        <v>1.95</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>2.0699999999999998</v>
+        <v>0.11</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>3.2000000000000001E-2</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>0.01</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>1.2E-2</v>
+        <v>0.01</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>5.0000000000000001E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>3.4</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>1E-3</v>
+        <v>3.4</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>7.57</v>
+        <v>1E-3</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>2.02</v>
+        <v>7.57</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>23.65</v>
+        <v>2.02</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>1.4</v>
+        <v>23.65</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>1.95</v>
+        <v>1.4</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>2.04</v>
+        <v>1.95</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>0.5</v>
+        <v>2.04</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>1.72</v>
+        <v>0.5</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>9.1</v>
+        <v>1.72</v>
       </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>4.0000000000000001E-3</v>
+        <v>9.1</v>
       </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B32">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="B33">
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>0.184</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>0.33</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>0.38</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>0.9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>0.38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>0.9</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>0.9</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <v>0.93</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>0.98</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>0.9</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>0.01</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>1</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>0.03</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>0.1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>0.184</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>0.33</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <v>0.15</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B55">
+      <c r="B56">
         <v>0.16</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B56">
+      <c r="B57">
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B57">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="B58">
         <v>0.7</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="B59">
         <v>0.7</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B60">
+      <c r="B61">
         <v>0.8</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B61">
+      <c r="B62">
         <v>0.34</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B62">
+      <c r="B63">
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B63">
+      <c r="B64">
         <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B64">
-        <v>0.41</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B65">
-        <v>0.8</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B66">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B67">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B68">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B69">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B70">
-        <v>0.6</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B71">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="B72">
         <v>0.8</v>
@@ -1780,31 +1789,31 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="B73">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B74">
-        <v>0.75</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B75">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B76">
         <v>0.7</v>
@@ -1812,14 +1821,22 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B77">
         <v>0.7</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="1"/>
+      <c r="A78" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Continuing edits for clarity prior to PR
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
   <si>
     <t>parameter_name</t>
   </si>
@@ -329,6 +329,21 @@
   </si>
   <si>
     <t>[0.04, 0.12, 0.80, 0.04]</t>
+  </si>
+  <si>
+    <t>odds_homebirth</t>
+  </si>
+  <si>
+    <t>or_homebirth_unmarried</t>
+  </si>
+  <si>
+    <t>or_homebirth_wealth_4</t>
+  </si>
+  <si>
+    <t>or_homebirth_wealth_5</t>
+  </si>
+  <si>
+    <t>or_homebirth_urban</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1204,9 +1219,6 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D5" s="2"/>
@@ -1246,15 +1258,12 @@
         <v>70</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>0.02</v>
       </c>
       <c r="C9">
-        <v>0.02</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E9">
         <v>0.09</v>
       </c>
     </row>
@@ -1661,79 +1670,79 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="B57">
-        <v>0.76100000000000001</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="B58">
-        <v>0.7</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="B59">
-        <v>0.7</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B60">
-        <v>0.7</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>92</v>
+      <c r="A61" t="s">
+        <v>107</v>
       </c>
       <c r="B61">
-        <v>0.8</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B62">
-        <v>0.34</v>
+        <v>0.76100000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B63">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B64">
-        <v>0.56999999999999995</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="B65">
-        <v>0.41</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="B66">
         <v>0.8</v>
@@ -1741,15 +1750,15 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B67">
-        <v>0.2</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B68">
         <v>0.5</v>
@@ -1757,86 +1766,126 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B69">
-        <v>0.3</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B70">
-        <v>0.15</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B71">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B72">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="B73">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B74">
-        <v>0.95</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B75">
-        <v>0.75</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B76">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B77">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B78">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B79">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B80">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B81">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B82">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B78">
+      <c r="B83">
         <v>0.7</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="1"/>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PR changes as requested
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -1167,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1179,7 +1179,7 @@
     <col min="2" max="2" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>88</v>
       </c>
@@ -1214,7 +1214,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1241,19 +1241,18 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <v>1.3</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" t="s">
+      <c r="D8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>101</v>
       </c>
@@ -1275,7 +1274,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>73</v>
       </c>
@@ -1284,7 +1283,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1293,7 +1292,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1302,7 +1301,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1311,7 +1310,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1320,7 +1319,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1601,18 +1600,15 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49">
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>45</v>
       </c>
@@ -1620,7 +1616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>46</v>
       </c>
@@ -1628,7 +1624,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>100</v>
       </c>
@@ -1636,7 +1632,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>48</v>
       </c>
@@ -1644,7 +1640,7 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>49</v>
       </c>
@@ -1652,7 +1648,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>50</v>
       </c>
@@ -1660,7 +1656,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>51</v>
       </c>
@@ -1668,7 +1664,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>103</v>
       </c>
@@ -1676,7 +1672,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>104</v>
       </c>
@@ -1684,7 +1680,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>105</v>
       </c>
@@ -1692,7 +1688,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>106</v>
       </c>
@@ -1700,7 +1696,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>107</v>
       </c>
@@ -1708,7 +1704,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>52</v>
       </c>
@@ -1716,7 +1712,7 @@
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>53</v>
       </c>
@@ -1724,7 +1720,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
Continued changes from PR review
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -1169,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
New branch with agreed changes to HSI structure
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="111">
   <si>
     <t>parameter_name</t>
   </si>
@@ -344,6 +344,15 @@
   </si>
   <si>
     <t>or_homebirth_urban</t>
+  </si>
+  <si>
+    <t>squeeze_factor_threshold_delivery_attendance</t>
+  </si>
+  <si>
+    <t>dummy_prob_health_centre</t>
+  </si>
+  <si>
+    <t>DUMMY</t>
   </si>
 </sst>
 </file>
@@ -1167,19 +1176,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.88671875" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1187,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1196,7 +1205,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -1205,7 +1214,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>88</v>
       </c>
@@ -1214,7 +1223,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1223,7 +1232,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1232,7 +1241,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1241,7 +1250,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1252,7 +1261,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -1266,7 +1275,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>101</v>
       </c>
@@ -1274,7 +1283,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>73</v>
       </c>
@@ -1283,7 +1292,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1292,7 +1301,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1301,7 +1310,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1310,7 +1319,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1319,7 +1328,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1328,7 +1337,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1337,7 +1346,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1346,7 +1355,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1355,7 +1364,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1364,7 +1373,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1373,7 +1382,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1382,7 +1391,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1391,7 +1400,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1400,7 +1409,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1409,7 +1418,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1418,7 +1427,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1427,7 +1436,7 @@
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1436,7 +1445,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1445,7 +1454,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1454,7 +1463,7 @@
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1463,7 +1472,7 @@
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
@@ -1472,7 +1481,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1480,7 +1489,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1488,7 +1497,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1496,7 +1505,7 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
@@ -1504,7 +1513,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
@@ -1512,7 +1521,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>95</v>
       </c>
@@ -1520,7 +1529,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -1528,7 +1537,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -1536,7 +1545,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -1544,7 +1553,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
@@ -1552,7 +1561,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>38</v>
       </c>
@@ -1560,7 +1569,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>98</v>
       </c>
@@ -1576,7 +1585,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>41</v>
       </c>
@@ -1584,7 +1593,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>42</v>
       </c>
@@ -1592,7 +1601,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
@@ -1600,7 +1609,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>44</v>
       </c>
@@ -1608,7 +1617,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>45</v>
       </c>
@@ -1616,7 +1625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>46</v>
       </c>
@@ -1624,7 +1633,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>100</v>
       </c>
@@ -1632,7 +1641,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>48</v>
       </c>
@@ -1640,7 +1649,7 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>49</v>
       </c>
@@ -1648,7 +1657,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>50</v>
       </c>
@@ -1656,7 +1665,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>51</v>
       </c>
@@ -1664,7 +1673,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>103</v>
       </c>
@@ -1672,7 +1681,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>104</v>
       </c>
@@ -1680,7 +1689,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>105</v>
       </c>
@@ -1688,7 +1697,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>106</v>
       </c>
@@ -1696,7 +1705,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>107</v>
       </c>
@@ -1704,7 +1713,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>52</v>
       </c>
@@ -1712,7 +1721,7 @@
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>53</v>
       </c>
@@ -1720,7 +1729,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>54</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>90</v>
       </c>
@@ -1736,7 +1745,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>92</v>
       </c>
@@ -1744,7 +1753,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>72</v>
       </c>
@@ -1752,7 +1761,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
@@ -1760,7 +1769,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>55</v>
       </c>
@@ -1768,7 +1777,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>56</v>
       </c>
@@ -1776,7 +1785,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>57</v>
       </c>
@@ -1784,7 +1793,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>58</v>
       </c>
@@ -1792,7 +1801,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>59</v>
       </c>
@@ -1800,7 +1809,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>60</v>
       </c>
@@ -1808,7 +1817,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>61</v>
       </c>
@@ -1816,7 +1825,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>62</v>
       </c>
@@ -1824,7 +1833,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>63</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>94</v>
       </c>
@@ -1840,7 +1849,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>64</v>
       </c>
@@ -1848,7 +1857,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>65</v>
       </c>
@@ -1856,7 +1865,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>66</v>
       </c>
@@ -1864,7 +1873,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>67</v>
       </c>
@@ -1872,7 +1881,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>68</v>
       </c>
@@ -1880,8 +1889,27 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B84">
+        <v>0.7</v>
+      </c>
+      <c r="C84" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B85">
+        <v>0.8</v>
+      </c>
+      <c r="C85" t="s">
+        <v>110</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1897,12 +1925,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1910,7 +1938,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1918,7 +1946,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -1926,7 +1954,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1934,7 +1962,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1942,7 +1970,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1950,7 +1978,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1958,7 +1986,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>70</v>
       </c>
@@ -1966,7 +1994,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
@@ -1974,7 +2002,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1982,7 +2010,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1990,7 +2018,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1998,7 +2026,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2006,7 +2034,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -2014,7 +2042,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -2022,7 +2050,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2030,7 +2058,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -2038,7 +2066,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -2046,7 +2074,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2054,7 +2082,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -2062,7 +2090,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -2070,7 +2098,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -2078,7 +2106,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -2089,7 +2117,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -2097,7 +2125,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2105,7 +2133,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -2113,7 +2141,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -2121,7 +2149,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -2129,7 +2157,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -2137,133 +2165,133 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
@@ -2271,17 +2299,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>90</v>
       </c>
@@ -2289,7 +2317,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>92</v>
       </c>
@@ -2297,17 +2325,17 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
@@ -2315,7 +2343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
@@ -2323,67 +2351,67 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
adding additional assert testing to main labour file
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -1181,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1231,9 +1231,6 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.15</v>
-      </c>
-      <c r="C5">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D5" s="2"/>

</xml_diff>

<commit_message>
new parameter not reading
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -1182,16 +1182,16 @@
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.88671875" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1208,7 +1208,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>88</v>
       </c>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>101</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>73</v>
       </c>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1304,7 +1304,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1412,7 +1412,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1475,7 +1475,7 @@
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>93</v>
       </c>
@@ -1484,7 +1484,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>33</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>95</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>34</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>36</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>38</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>98</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>41</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>42</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>44</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>45</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>46</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>100</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>48</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>49</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>50</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>51</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>103</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>104</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>1.83</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>105</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>106</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>107</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>52</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>53</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>54</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>90</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>111</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>92</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>72</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>74</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>55</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>56</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>57</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>58</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>59</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>60</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>61</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>62</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>63</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>94</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>64</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>65</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>66</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>67</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>68</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>109</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>108</v>
       </c>
@@ -1936,12 +1936,12 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>70</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>73</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
@@ -2176,133 +2176,133 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>52</v>
       </c>
@@ -2310,17 +2310,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>90</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>92</v>
       </c>
@@ -2336,17 +2336,17 @@
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
@@ -2362,67 +2362,67 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
merged in changes from submitted PR and ongoing work on HSIs
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
   <si>
     <t>parameter_name</t>
   </si>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>rr_sepsis_post_abx_pprom</t>
+  </si>
+  <si>
+    <t>squeeze_factor_threshold_sba_did_not_run</t>
   </si>
 </sst>
 </file>
@@ -1179,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,6 +1923,14 @@
       </c>
       <c r="C86" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B87">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding dx testing and AVD to first SBA HSI
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -13,14 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="parameter_sources" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="124">
   <si>
     <t>parameter_name</t>
   </si>
@@ -46,9 +46,6 @@
     <t>rr_PL_OL_nuliparity</t>
   </si>
   <si>
-    <t>rr_PL_OL_para1</t>
-  </si>
-  <si>
     <t>rr_PL_OL_age_less20</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>Malawi Demographic and Health Survey (2010)</t>
   </si>
   <si>
-    <t>Individual and health facility factors and the risk for obstructed labour and its adverse outcomes in south-western Uganda (Kabakyenga et al. 2011)</t>
-  </si>
-  <si>
     <t>Global, regional, and national estimates of levels of preterm birth in 2014: a systematic review and modelling analysis (Chawanpaiboon et al 2019)</t>
   </si>
   <si>
@@ -361,20 +355,50 @@
     <t>squeeze_factor_threshold_sba_did_not_run</t>
   </si>
   <si>
-    <t>sensitivity_of_assessment_of_obstructed_labour</t>
-  </si>
-  <si>
-    <t>sensitivity_of_assessment_of_sepsis</t>
-  </si>
-  <si>
-    <t>sensitivity_of_assessment_of_uterine_rupture</t>
+    <t>sensitivity_of_assessment_of_obstructed_labour_hc</t>
+  </si>
+  <si>
+    <t>sensitivity_of_assessment_of_obstructed_labour_hp</t>
+  </si>
+  <si>
+    <t>sensitivity_of_assessment_of_sepsis_hc</t>
+  </si>
+  <si>
+    <t>sensitivity_of_assessment_of_sepsis_hp</t>
+  </si>
+  <si>
+    <t>sensitivity_of_assessment_of_uterine_rupture_hc</t>
+  </si>
+  <si>
+    <t>sensitivity_of_assessment_of_uterine_rupture_hp</t>
+  </si>
+  <si>
+    <t>sensitivity_of_assessment_of_obstructed_labour_for_cs</t>
+  </si>
+  <si>
+    <t>rr_PL_OL_bmi_less18</t>
+  </si>
+  <si>
+    <t>rr_PL_OL_bmi_more25</t>
+  </si>
+  <si>
+    <t>rr_PL_OL_para_more3</t>
+  </si>
+  <si>
+    <t>A prospective population-based study of maternal, fetal, and neonatal outcomes in the setting of prolonged labor, obstructed labor and failure to progress in low- and middle-income countries (Harrison et al 2015)</t>
+  </si>
+  <si>
+    <t>value type</t>
+  </si>
+  <si>
+    <t>Relative Risk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,6 +536,22 @@
     <font>
       <b/>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -860,7 +900,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -870,6 +910,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1191,15 +1236,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90:XFD90"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="1" max="1" width="52.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1213,7 +1258,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B2">
         <v>8.3000000000000004E-2</v>
@@ -1222,7 +1267,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B3">
         <v>4.5999999999999999E-2</v>
@@ -1231,7 +1276,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>0.03</v>
@@ -1258,503 +1303,503 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="B7">
-        <v>1.57</v>
+        <v>0.8</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="B8">
-        <v>1.3</v>
+        <v>0.8</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="B9">
-        <v>0.02</v>
-      </c>
-      <c r="C9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="D9">
-        <v>0.09</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>102</v>
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1.3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B11">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>0.02</v>
+      </c>
+      <c r="C11">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D11">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>1.73</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="B13">
-        <v>2.63</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14">
-        <v>1.95</v>
+        <v>1.73</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15">
-        <v>0.11</v>
+        <v>2.63</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16">
-        <v>2.0699999999999998</v>
+        <v>1.95</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>3.2000000000000001E-2</v>
+        <v>0.11</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18">
-        <v>0.01</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19">
-        <v>1.2E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>3.4</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>1E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23">
-        <v>7.57</v>
+        <v>3.4</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B24">
-        <v>2.02</v>
+        <v>1E-3</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25">
-        <v>23.65</v>
+        <v>7.57</v>
       </c>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26">
-        <v>1.4</v>
+        <v>2.02</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27">
-        <v>1.95</v>
+        <v>23.65</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B28">
-        <v>2.04</v>
+        <v>1.4</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29">
-        <v>0.5</v>
+        <v>1.95</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30">
-        <v>1.72</v>
+        <v>2.04</v>
       </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31">
-        <v>9.1</v>
+        <v>0.5</v>
       </c>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>1.72</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33">
+        <v>9.1</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39">
+        <v>0.34499999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B32">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35">
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37">
-        <v>0.34499999999999997</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="B40">
         <v>0.38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B41">
         <v>0.9</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B42">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B43">
         <v>0.9</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="B44">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46">
         <v>0.93</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47">
         <v>0.98</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48">
         <v>0.03</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48">
-        <v>0.01</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B49">
-        <v>0.03</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B51">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="B52">
-        <v>0.1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B53">
-        <v>0.184</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="B54">
-        <v>0.33</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B55">
-        <v>0.15</v>
+        <v>0.184</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B56">
-        <v>0.16</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="B57">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="B58">
-        <v>1.83</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B59">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B60">
-        <v>0.43</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>107</v>
+      <c r="A61" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="B61">
-        <v>0.39</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="B62">
-        <v>0.76100000000000001</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>53</v>
+      <c r="A63" t="s">
+        <v>105</v>
       </c>
       <c r="B63">
-        <v>0.7</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B64">
-        <v>0.7</v>
+        <v>0.76100000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B65">
         <v>0.7</v>
@@ -1762,7 +1807,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="B66">
         <v>0.7</v>
@@ -1770,143 +1815,143 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B67">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="B68">
-        <v>0.34</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B69">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B70">
-        <v>0.56999999999999995</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="B71">
-        <v>0.41</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B72">
-        <v>0.8</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B73">
-        <v>0.2</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B74">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B75">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B76">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B77">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B78">
-        <v>0.8</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="B79">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B80">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="B81">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B82">
-        <v>0.7</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B83">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B84">
         <v>0.7</v>
@@ -1914,68 +1959,128 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="B85">
         <v>0.7</v>
       </c>
-      <c r="C85" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="B86">
-        <v>0.8</v>
-      </c>
-      <c r="C86" t="s">
-        <v>110</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B87">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="C87" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B88">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C88" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B89">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="C89" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B90">
+        <v>0.25</v>
+      </c>
+      <c r="C90" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B91">
+        <v>0.5</v>
+      </c>
+      <c r="C91" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B92">
+        <v>0.8</v>
+      </c>
+      <c r="C92" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B93">
+        <v>0.5</v>
+      </c>
+      <c r="C93" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B94">
+        <v>0.25</v>
+      </c>
+      <c r="C94" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B90">
+      <c r="B95">
         <v>0.7</v>
       </c>
-      <c r="C90" t="s">
-        <v>110</v>
+      <c r="C95" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B96">
+        <v>0.35</v>
+      </c>
+      <c r="C96" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1986,39 +2091,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>75</v>
+      <c r="B1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,464 +2135,496 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B5" s="5" t="s">
+        <v>123</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>120</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>118</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>70</v>
+        <v>119</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B55" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B58" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B59" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>72</v>
+        <v>88</v>
+      </c>
+      <c r="B60" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>74</v>
+        <v>90</v>
+      </c>
+      <c r="B61" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B62" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B63" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
requested changes from Tim H
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="114">
   <si>
     <t>parameter_name</t>
   </si>
@@ -344,6 +344,24 @@
   </si>
   <si>
     <t>or_homebirth_urban</t>
+  </si>
+  <si>
+    <t>parity_unit_age_increase</t>
+  </si>
+  <si>
+    <t>parity_marriage_level_2</t>
+  </si>
+  <si>
+    <t>parity_marriage_level_3</t>
+  </si>
+  <si>
+    <t>parity_constant_value</t>
+  </si>
+  <si>
+    <t>parity_by_wealth_level</t>
+  </si>
+  <si>
+    <t>[-0.9,-0.37,-0.26,-0.13,-0.13]</t>
   </si>
 </sst>
 </file>
@@ -1167,19 +1185,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.88671875" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1187,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1196,7 +1214,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>96</v>
       </c>
@@ -1205,683 +1223,733 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4">
+        <v>-3</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5">
+        <v>0.22</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6">
+        <v>0.91</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7">
+        <v>0.16</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B4">
+      <c r="B9">
         <v>0.03</v>
       </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B10">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
+      <c r="B11">
         <v>1.47</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B12">
         <v>1.57</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B13">
         <v>1.3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14">
+        <v>0.02</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>1.73</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>2.63</v>
+      </c>
+      <c r="D18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>1.95</v>
+      </c>
+      <c r="C19">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23">
+        <v>0.01</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26">
+        <v>3.4</v>
+      </c>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>1E-3</v>
+      </c>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <v>7.57</v>
+      </c>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29">
+        <v>2.02</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <v>23.65</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>1.4</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>1.95</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33">
+        <v>2.04</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35">
+        <v>1.72</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36">
+        <v>9.1</v>
+      </c>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38">
         <v>0.02</v>
       </c>
-      <c r="C9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="D9">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>1.73</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>2.63</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>1.95</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>0.11</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39">
+        <v>0.02</v>
+      </c>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40">
+        <v>0.184</v>
+      </c>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41">
+        <v>0.33</v>
+      </c>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53">
         <v>0.01</v>
       </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>1.2E-2</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>3.4</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>1E-3</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>7.57</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>2.02</v>
-      </c>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>23.65</v>
-      </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>1.4</v>
-      </c>
-      <c r="D26" s="2"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27">
-        <v>1.95</v>
-      </c>
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>2.04</v>
-      </c>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B59">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62">
         <v>0.5</v>
       </c>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30">
-        <v>1.72</v>
-      </c>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31">
-        <v>9.1</v>
-      </c>
-      <c r="D31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B32">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35">
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37">
-        <v>0.34499999999999997</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B38">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B49">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B52">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53">
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B54">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B55">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B58">
+      <c r="B63">
         <v>1.83</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B59">
+      <c r="B64">
         <v>0.51</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B60">
+      <c r="B65">
         <v>0.43</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>107</v>
       </c>
-      <c r="B61">
+      <c r="B66">
         <v>0.39</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B62">
+      <c r="B67">
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B63">
+      <c r="B68">
         <v>0.7</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B64">
+      <c r="B69">
         <v>0.7</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B65">
+      <c r="B70">
         <v>0.7</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B66">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B67">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B68">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B69">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B70">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="B71">
         <v>0.8</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B72">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B73">
         <v>0.5</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B74">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B75">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B76">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B77">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B78">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B74">
+      <c r="B79">
         <v>0.3</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B75">
+      <c r="B80">
         <v>0.15</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B76">
+      <c r="B81">
         <v>0.6</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B77">
+      <c r="B82">
         <v>0.8</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B78">
+      <c r="B83">
         <v>0.8</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B79">
+      <c r="B84">
         <v>0.95</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B80">
+      <c r="B85">
         <v>0.75</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B81">
+      <c r="B86">
         <v>0.7</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B82">
+      <c r="B87">
         <v>0.7</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B83">
+      <c r="B88">
         <v>0.7</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1891,18 +1959,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1910,7 +1978,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
@@ -1918,7 +1986,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -1926,465 +1994,495 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B28" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B63" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B64" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B67" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B68" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reformatting death event so that the linear model is used to calculate individual risk of death. Treatment effect is incoprerated as a predictor of death
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="130">
   <si>
     <t>parameter_name</t>
   </si>
@@ -310,9 +310,6 @@
     <t>prob_still_birth_uterine_rupture</t>
   </si>
   <si>
-    <t>prob_still_birth_uterine_rupture_md</t>
-  </si>
-  <si>
     <t xml:space="preserve">correct: </t>
   </si>
   <si>
@@ -410,6 +407,9 @@
   </si>
   <si>
     <t>sensitivity_of_treatment_assessment_of_antepartum_haem_hp</t>
+  </si>
+  <si>
+    <t>prob_still_birth_antepartum_haem</t>
   </si>
 </sst>
 </file>
@@ -1254,19 +1254,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>94</v>
       </c>
@@ -1292,7 +1292,7 @@
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -1301,7 +1301,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1319,35 +1319,35 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7">
         <v>0.8</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B8">
         <v>0.8</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B9">
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
@@ -1369,15 +1369,15 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>72</v>
       </c>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1458,7 +1458,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>18</v>
       </c>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1503,7 +1503,7 @@
       </c>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1539,7 +1539,7 @@
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>91</v>
       </c>
@@ -1575,23 +1575,29 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B35">
+        <v>0.15</v>
+      </c>
+      <c r="C35">
         <v>0.02</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B36">
+        <v>0.15</v>
+      </c>
+      <c r="C36">
         <v>0.02</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
@@ -1599,7 +1605,7 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>70</v>
       </c>
@@ -1607,7 +1613,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>32</v>
       </c>
@@ -1615,7 +1621,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>93</v>
       </c>
@@ -1623,548 +1629,508 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="B41">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B42">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="B43">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B44">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B45">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="B46">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B48">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="B49">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B50">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B51">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B53">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B54">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="B55">
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="B56">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="B57">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>50</v>
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>104</v>
       </c>
       <c r="B58">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B59">
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B62">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B63">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66">
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B60">
-        <v>1.83</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B61">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B62">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>105</v>
-      </c>
-      <c r="B63">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B64">
-        <v>0.76100000000000001</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B65">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="B67">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="B68">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="B69">
         <v>0.8</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B70">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B71">
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B72">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B73">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B74">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B75">
         <v>0.8</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B75">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="B76">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B77">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B78">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B79">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B81">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82">
+        <v>0.7</v>
+      </c>
+      <c r="C82" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B83">
+        <v>0.8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B84">
+        <v>0.9</v>
+      </c>
+      <c r="C84" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B85">
+        <v>0.25</v>
+      </c>
+      <c r="C85" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B86">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B77">
+      <c r="C86" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B87">
+        <v>0.8</v>
+      </c>
+      <c r="C87" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B88">
+        <v>0.5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B89">
+        <v>0.25</v>
+      </c>
+      <c r="C89" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B90">
+        <v>0.4</v>
+      </c>
+      <c r="C90" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B91">
+        <v>0.8</v>
+      </c>
+      <c r="C91" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B92">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B78">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B79">
+      <c r="C92" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B93">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B80">
+      <c r="C93" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B94">
+        <v>0.4</v>
+      </c>
+      <c r="C94" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B95">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B81">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B82">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B83">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B84">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B85">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B86">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="C95" t="s">
         <v>107</v>
       </c>
-      <c r="B87">
-        <v>0.7</v>
-      </c>
-      <c r="C87" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B88">
-        <v>0.8</v>
-      </c>
-      <c r="C88" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B89">
-        <v>0.9</v>
-      </c>
-      <c r="C89" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B90">
-        <v>0.25</v>
-      </c>
-      <c r="C90" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B91">
-        <v>0.5</v>
-      </c>
-      <c r="C91" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B92">
-        <v>0.8</v>
-      </c>
-      <c r="C92" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B93">
-        <v>0.5</v>
-      </c>
-      <c r="C93" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B94">
-        <v>0.25</v>
-      </c>
-      <c r="C94" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B95">
-        <v>0.4</v>
-      </c>
-      <c r="C95" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B96">
+        <v>0.5</v>
+      </c>
+      <c r="C96" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B97">
         <v>0.8</v>
       </c>
-      <c r="C96" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B97">
-        <v>0.3</v>
-      </c>
       <c r="C97" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B98">
-        <v>0.6</v>
-      </c>
-      <c r="C98" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B99">
-        <v>0.4</v>
-      </c>
-      <c r="C99" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B100">
-        <v>0.8</v>
-      </c>
-      <c r="C100" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B101">
-        <v>0.5</v>
-      </c>
-      <c r="C101" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B102">
-        <v>0.8</v>
-      </c>
-      <c r="C102" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2181,24 +2147,24 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -2206,7 +2172,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>86</v>
       </c>
@@ -2214,70 +2180,70 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="B8" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
@@ -2285,7 +2251,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>72</v>
       </c>
@@ -2293,7 +2259,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -2301,7 +2267,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2309,7 +2275,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -2317,7 +2283,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -2325,7 +2291,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2333,7 +2299,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2341,7 +2307,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2349,7 +2315,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -2357,7 +2323,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -2365,7 +2331,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -2373,7 +2339,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2381,7 +2347,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -2389,7 +2355,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -2397,7 +2363,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
@@ -2408,7 +2374,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -2416,7 +2382,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -2424,7 +2390,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -2432,7 +2398,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -2440,7 +2406,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -2448,7 +2414,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -2456,133 +2422,133 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
@@ -2590,17 +2556,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>88</v>
       </c>
@@ -2608,7 +2574,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>90</v>
       </c>
@@ -2616,17 +2582,17 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>54</v>
       </c>
@@ -2634,7 +2600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>55</v>
       </c>
@@ -2642,67 +2608,67 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
first draft of postpartum event
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="137">
   <si>
     <t>parameter_name</t>
   </si>
@@ -413,6 +413,24 @@
   </si>
   <si>
     <t>prob_successful_assisted_vaginal_delivery</t>
+  </si>
+  <si>
+    <t>severity_maternal_haemorrhage</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>[0.3, 0.7]</t>
+  </si>
+  <si>
+    <t>prob_pph_source</t>
+  </si>
+  <si>
+    <t>[0.67, 0.33]</t>
+  </si>
+  <si>
+    <t>prob_successful_manual_removal_placenta</t>
   </si>
 </sst>
 </file>
@@ -1257,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1571,59 +1589,72 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34">
-        <v>4.0000000000000001E-3</v>
+        <v>131</v>
+      </c>
+      <c r="B34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" t="s">
+        <v>132</v>
       </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="B35">
-        <v>0.15</v>
-      </c>
-      <c r="C35">
-        <v>0.02</v>
-      </c>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36">
-        <v>0.184</v>
+        <v>0.6</v>
+      </c>
+      <c r="C36">
+        <v>0.02</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="B37">
-        <v>0.33</v>
+        <v>0.5</v>
+      </c>
+      <c r="C37">
+        <v>0.184</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B38">
-        <v>0.34499999999999997</v>
+        <v>0.5</v>
+      </c>
+      <c r="C38">
+        <v>0.33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="B39">
-        <v>0.38</v>
+        <v>0.8</v>
+      </c>
+      <c r="C39">
+        <v>0.34499999999999997</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="B40">
         <v>0.38</v>
@@ -1631,344 +1662,347 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="B41">
-        <v>0.25</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="B42">
-        <v>0.93</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>40</v>
+        <v>95</v>
       </c>
       <c r="B43">
-        <v>0.03</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B44">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>0.05</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B48">
+      <c r="B50">
+        <v>0.5</v>
+      </c>
+      <c r="C50">
         <v>0.1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B49">
+      <c r="B51">
+        <v>0.5</v>
+      </c>
+      <c r="C51">
         <v>0.184</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
+      <c r="B52">
+        <v>0.5</v>
+      </c>
+      <c r="C52">
         <v>0.33</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B51">
+      <c r="B53">
         <v>0.15</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B52">
+      <c r="B54">
         <v>0.16</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B53">
+      <c r="B55">
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B54">
+      <c r="B56">
         <v>1.83</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B55">
+      <c r="B57">
         <v>0.51</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B56">
+      <c r="B58">
         <v>0.43</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>104</v>
       </c>
-      <c r="B57">
+      <c r="B59">
         <v>0.39</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B58">
+      <c r="B60">
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B59">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B60">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="B61">
         <v>0.7</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="B62">
         <v>0.7</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B63">
+      <c r="B65">
         <v>0.8</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B64">
+      <c r="B66">
         <v>0.34</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B65">
+      <c r="B67">
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B66">
+      <c r="B68">
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B67">
+      <c r="B69">
         <v>0.41</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B68">
+      <c r="B70">
         <v>0.8</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B69">
+      <c r="B71">
         <v>0.2</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B70">
+      <c r="B72">
         <v>0.5</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B71">
+      <c r="B73">
         <v>0.3</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B72">
+      <c r="B74">
         <v>0.15</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B73">
+      <c r="B75">
         <v>0.6</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B74">
+      <c r="B76">
         <v>0.8</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B75">
+      <c r="B77">
         <v>0.8</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B76">
+      <c r="B78">
         <v>0.95</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B77">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B79">
         <v>0.75</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B78">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>130</v>
-      </c>
-      <c r="B79">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="B80">
         <v>0.7</v>
       </c>
-      <c r="C80" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>105</v>
+      <c r="A81" t="s">
+        <v>130</v>
       </c>
       <c r="B81">
-        <v>0.8</v>
-      </c>
-      <c r="C81" t="s">
-        <v>107</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B82">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="C82" t="s">
         <v>107</v>
@@ -1976,10 +2010,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B83">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="C83" t="s">
         <v>107</v>
@@ -1987,10 +2021,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B84">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="C84" t="s">
         <v>107</v>
@@ -1998,10 +2032,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B85">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="C85" t="s">
         <v>107</v>
@@ -2009,7 +2043,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B86">
         <v>0.5</v>
@@ -2020,10 +2054,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B87">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="C87" t="s">
         <v>107</v>
@@ -2031,10 +2065,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B88">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="C88" t="s">
         <v>107</v>
@@ -2042,10 +2076,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B89">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="C89" t="s">
         <v>107</v>
@@ -2053,10 +2087,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B90">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="C90" t="s">
         <v>107</v>
@@ -2064,10 +2098,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B91">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="C91" t="s">
         <v>107</v>
@@ -2075,10 +2109,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B92">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C92" t="s">
         <v>107</v>
@@ -2086,10 +2120,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B93">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C93" t="s">
         <v>107</v>
@@ -2097,10 +2131,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B94">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C94" t="s">
         <v>107</v>
@@ -2108,12 +2142,34 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B95">
         <v>0.8</v>
       </c>
       <c r="C95" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B96">
+        <v>0.5</v>
+      </c>
+      <c r="C96" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B97">
+        <v>0.8</v>
+      </c>
+      <c r="C97" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2127,8 +2183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
starting work on reformmating newborn epi
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -978,7 +978,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -989,6 +989,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1312,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,8 +1701,8 @@
       <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B44">
-        <v>0.15</v>
+      <c r="B44" s="6">
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new linear equations for care-seeking
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -15,7 +15,7 @@
     <sheet name="parameter_values" sheetId="1" r:id="rId1"/>
     <sheet name="parameter_sources" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -25,7 +25,7 @@
     <author>Joseph Collins</author>
   </authors>
   <commentList>
-    <comment ref="D51" authorId="0" shapeId="0">
+    <comment ref="D67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="150">
   <si>
     <t>parameter_name</t>
   </si>
@@ -457,6 +457,54 @@
   </si>
   <si>
     <t>or_comp_careseeking_wealth_2</t>
+  </si>
+  <si>
+    <t>odds_deliver_in_health_centre</t>
+  </si>
+  <si>
+    <t>rrr_hc_delivery_age_25_29</t>
+  </si>
+  <si>
+    <t>rrr_hc_delivery_age_30_34</t>
+  </si>
+  <si>
+    <t>rrr_hc_delivery_age_35_39</t>
+  </si>
+  <si>
+    <t>rrr_hc_delivery_age_40_44</t>
+  </si>
+  <si>
+    <t>rrr_hc_delivery_age_45_49</t>
+  </si>
+  <si>
+    <t>rrr_hc_delivery_parity_3_to_4</t>
+  </si>
+  <si>
+    <t>rrr_hc_delivery_parity_&gt;4</t>
+  </si>
+  <si>
+    <t>rrr_hc_delivery_married</t>
+  </si>
+  <si>
+    <t>rrr_hc_delivery_rural</t>
+  </si>
+  <si>
+    <t>odds_deliver_at_home</t>
+  </si>
+  <si>
+    <t>rrr_hb_delivery_age_35_39</t>
+  </si>
+  <si>
+    <t>rrr_hb_delivery_age_40_44</t>
+  </si>
+  <si>
+    <t>rrr_hb_delivery_age_45_49</t>
+  </si>
+  <si>
+    <t>rrr_hb_delivery_parity_3_to_4</t>
+  </si>
+  <si>
+    <t>rrr_hb_delivery_parity_&gt;4</t>
   </si>
 </sst>
 </file>
@@ -1313,10 +1361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +1440,10 @@
         <v>70</v>
       </c>
       <c r="B8">
-        <v>1.0999999999999999E-2</v>
+        <v>0.01</v>
+      </c>
+      <c r="C8">
+        <v>2.3E-2</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -1419,7 +1470,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.11</v>
+        <v>0.05</v>
+      </c>
+      <c r="C11">
+        <v>0.1</v>
       </c>
       <c r="D11" s="2"/>
     </row>
@@ -1737,7 +1791,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>95</v>
       </c>
@@ -1745,7 +1799,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -1753,286 +1807,414 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>136</v>
+      </c>
+      <c r="B53">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>138</v>
+      </c>
+      <c r="B55">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>140</v>
+      </c>
+      <c r="B58">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>141</v>
+      </c>
+      <c r="B59">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>142</v>
+      </c>
+      <c r="B60">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>146</v>
+      </c>
+      <c r="B63">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>147</v>
+      </c>
+      <c r="B64">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B65">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>149</v>
+      </c>
+      <c r="B66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B51">
+      <c r="B67">
         <v>1.08</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D67" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>133</v>
       </c>
-      <c r="B52">
+      <c r="B68">
         <v>2.5</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B53">
+      <c r="B69">
         <v>0.76100000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B54">
+      <c r="B70">
         <v>0.7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B55">
+      <c r="B71">
         <v>0.7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B56">
+      <c r="B72">
         <v>0.7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B57">
+      <c r="B73">
         <v>0.7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B58">
+      <c r="B74">
         <v>0.8</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B59">
+      <c r="B75">
         <v>0.34</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B60">
+      <c r="B76">
         <v>0.7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B61">
+      <c r="B77">
         <v>0.75</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B62">
+      <c r="B78">
         <v>0.7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>122</v>
       </c>
-      <c r="B63">
+      <c r="B79">
         <v>0.7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B64">
-        <v>0.7</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B80">
+        <v>0.4</v>
+      </c>
+      <c r="C80" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B65">
+      <c r="B81">
         <v>0.8</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C81" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B66">
+      <c r="B82">
         <v>0.9</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C82" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B67">
+      <c r="B83">
         <v>0.25</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C83" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B68">
+      <c r="B84">
         <v>0.5</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C84" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B69">
+      <c r="B85">
         <v>0.8</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C85" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B70">
+      <c r="B86">
         <v>0.5</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C86" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B71">
+      <c r="B87">
         <v>0.25</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C87" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B72">
+      <c r="B88">
         <v>0.4</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C88" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B73">
+      <c r="B89">
         <v>0.8</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C89" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B74">
+      <c r="B90">
         <v>0.3</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C90" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B75">
+      <c r="B91">
         <v>0.6</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C91" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B76">
+      <c r="B92">
         <v>0.4</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C92" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B77">
+      <c r="B93">
         <v>0.8</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C93" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B78">
+      <c r="B94">
         <v>0.5</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C94" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B79">
+      <c r="B95">
         <v>0.8</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C95" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edits to newborn linear models
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6405" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6408" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="139">
   <si>
     <t>parameter_name</t>
   </si>
@@ -468,6 +468,9 @@
   </si>
   <si>
     <t>cfr_severe_pre_eclamp</t>
+  </si>
+  <si>
+    <t>success_rate_surgical_removal_placenta</t>
   </si>
 </sst>
 </file>
@@ -1304,19 +1307,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>93</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>95</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>96</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>97</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>98</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>99</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1438,7 +1441,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1468,7 +1471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -1482,7 +1485,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -1496,7 +1499,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>110</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>111</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>113</v>
       </c>
@@ -1564,7 +1567,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>114</v>
       </c>
@@ -1576,7 +1579,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>115</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>116</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>117</v>
       </c>
@@ -1612,7 +1615,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>126</v>
       </c>
@@ -1651,7 +1654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>127</v>
       </c>
@@ -1666,7 +1669,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>128</v>
       </c>
@@ -1681,7 +1684,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>129</v>
       </c>
@@ -1696,7 +1699,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>130</v>
       </c>
@@ -1711,7 +1714,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>131</v>
       </c>
@@ -1738,7 +1741,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>132</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>133</v>
       </c>
@@ -1768,7 +1771,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>134</v>
       </c>
@@ -1783,7 +1786,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
@@ -1795,7 +1798,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>62</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>137</v>
       </c>
@@ -1826,7 +1829,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -1834,7 +1837,7 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>23</v>
       </c>
@@ -1842,7 +1845,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>11</v>
       </c>
@@ -1850,7 +1853,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
@@ -1858,7 +1861,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>60</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>12</v>
       </c>
@@ -1874,7 +1877,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>36</v>
       </c>
@@ -1882,7 +1885,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>136</v>
       </c>
@@ -1890,7 +1893,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>13</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>14</v>
       </c>
@@ -1906,7 +1909,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>15</v>
       </c>
@@ -1914,7 +1917,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>16</v>
       </c>
@@ -1925,7 +1928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>65</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>118</v>
       </c>
@@ -1944,7 +1947,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>120</v>
       </c>
@@ -1958,7 +1961,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>121</v>
       </c>
@@ -1972,7 +1975,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>122</v>
       </c>
@@ -1986,7 +1989,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>123</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>124</v>
       </c>
@@ -2014,7 +2017,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>125</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>37</v>
       </c>
@@ -2036,7 +2039,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
@@ -2044,7 +2047,7 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>18</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>19</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>6.2E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>20</v>
       </c>
@@ -2068,7 +2071,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>73</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -2087,7 +2090,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -2095,7 +2098,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>78</v>
       </c>
@@ -2119,7 +2122,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -2135,7 +2138,7 @@
         <v>2.21</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -2143,7 +2146,7 @@
         <v>4.3600000000000003</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -2151,7 +2154,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>83</v>
       </c>
@@ -2162,7 +2165,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -2170,7 +2173,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>86</v>
       </c>
@@ -2186,7 +2189,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>87</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>88</v>
       </c>
@@ -2202,7 +2205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>70</v>
       </c>
@@ -2213,7 +2216,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>72</v>
       </c>
@@ -2221,7 +2224,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>21</v>
       </c>
@@ -2229,7 +2232,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>22</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>33</v>
       </c>
@@ -2245,7 +2248,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>41</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>34</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>24</v>
       </c>
@@ -2269,7 +2272,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>69</v>
       </c>
@@ -2277,203 +2280,211 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B91">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B91">
+      <c r="B92">
         <v>0.75</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B92">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>61</v>
       </c>
       <c r="B93">
         <v>0.7</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>61</v>
+      </c>
+      <c r="B94">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B94">
+      <c r="B95">
         <v>0.4</v>
-      </c>
-      <c r="C94" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B95">
-        <v>0.8</v>
       </c>
       <c r="C95" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B96">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="C96" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B97">
-        <v>0.25</v>
+        <v>0.9</v>
       </c>
       <c r="C97" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B98">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C98" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B99">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="C99" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B100">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C100" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B101">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="C101" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B102">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="C102" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B103">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="C103" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B104">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="C104" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B105">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="C105" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B106">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="C106" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B107">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="C107" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B108">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C108" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B109">
+        <v>0.5</v>
+      </c>
+      <c r="C109" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B109">
+      <c r="B110">
         <v>0.8</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating testing and parameters
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6408" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6405" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <author>Joseph Collins</author>
   </authors>
   <commentList>
-    <comment ref="D82" authorId="0" shapeId="0">
+    <comment ref="D87" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="160">
   <si>
     <t>parameter_name</t>
   </si>
@@ -173,9 +173,6 @@
     <t>squeeze_factor_threshold_delivery_attendance</t>
   </si>
   <si>
-    <t>dummy_prob_health_centre</t>
-  </si>
-  <si>
     <t>DUMMY</t>
   </si>
   <si>
@@ -471,6 +468,72 @@
   </si>
   <si>
     <t>success_rate_surgical_removal_placenta</t>
+  </si>
+  <si>
+    <t>obstructed_labour_delayed_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>obstructed_labour_prompt_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>rr_still_birth_ol_maternal_death</t>
+  </si>
+  <si>
+    <t>sepsis_delayed_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>sepsis_prompt_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>sepsis_delayed_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>sepsis_prompt_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>eclampsia_treatment_effect_severe_pe</t>
+  </si>
+  <si>
+    <t>eclampsia_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>rr_still_birth_sepsis_maternal_death</t>
+  </si>
+  <si>
+    <t>rr_still_birth_eclampsia_maternal_death</t>
+  </si>
+  <si>
+    <t>eclampsia_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>aph_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>aph_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>aph_bt_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>rr_still_birth_aph_maternal_death</t>
+  </si>
+  <si>
+    <t>pph_delayed_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>pph_prompt_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>pph_bt_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>ur_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>ur_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>rr_still_birth_ur_maternal_death</t>
   </si>
 </sst>
 </file>
@@ -976,7 +1039,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -986,6 +1049,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1307,19 +1373,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G110"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1327,109 +1393,109 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2">
         <v>-3</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3">
         <v>0.22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4">
         <v>0.91</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5">
         <v>0.16</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6">
         <v>-0.13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7">
         <v>-0.13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8">
         <v>-0.26</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9">
         <v>-0.37</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10">
         <v>-0.9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1438,84 +1504,69 @@
       </c>
       <c r="D11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
         <v>1.47</v>
       </c>
       <c r="D12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
         <v>0.8</v>
       </c>
       <c r="D13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>0.8</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>0.8</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
         <v>1.4</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
         <v>1.3</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B17">
         <v>0.01</v>
@@ -1528,9 +1579,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18">
         <v>1.73</v>
@@ -1540,9 +1591,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B19">
         <v>2.63</v>
@@ -1552,9 +1603,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B20">
         <v>0.05</v>
@@ -1567,9 +1618,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B21">
         <v>2.0699999999999998</v>
@@ -1579,9 +1630,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22">
         <v>3.2000000000000001E-2</v>
@@ -1591,9 +1642,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B23">
         <v>3.88</v>
@@ -1603,9 +1654,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B24">
         <v>2.4</v>
@@ -1615,7 +1666,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -1627,14 +1678,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
         <v>3.4</v>
       </c>
       <c r="D26" s="2"/>
@@ -1642,9 +1690,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27">
         <v>0.01</v>
@@ -1654,14 +1702,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
         <v>1.4</v>
       </c>
       <c r="D28" s="2"/>
@@ -1669,14 +1714,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
         <v>1.95</v>
       </c>
       <c r="D29" s="2"/>
@@ -1684,14 +1726,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
         <v>2.04</v>
       </c>
       <c r="D30" s="2"/>
@@ -1699,14 +1738,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31">
         <v>2</v>
       </c>
       <c r="D31" s="2"/>
@@ -1714,7 +1750,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1726,9 +1762,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B33">
         <v>0.01</v>
@@ -1738,79 +1774,67 @@
       </c>
       <c r="D33" s="2"/>
       <c r="G33" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34">
         <v>7.57</v>
       </c>
       <c r="D34" s="2"/>
       <c r="G34" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35">
         <v>2.02</v>
       </c>
       <c r="D35" s="2"/>
       <c r="G35" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36">
         <v>23.65</v>
       </c>
       <c r="D36" s="2"/>
       <c r="G36" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37">
         <v>9.1</v>
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D38" s="2"/>
       <c r="G38" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>9</v>
       </c>
@@ -1818,18 +1842,18 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B40">
         <v>0.184</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -1837,7 +1861,7 @@
         <v>0.184</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>23</v>
       </c>
@@ -1845,7 +1869,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>11</v>
       </c>
@@ -1853,7 +1877,7 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
@@ -1861,631 +1885,826 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="B45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46">
         <v>0.38</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B46">
+      <c r="B48">
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+    <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B47">
+      <c r="B50">
         <v>0.93</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B48">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B52">
         <v>0.38</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B49">
+      <c r="B53">
         <v>0.03</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B50">
+      <c r="B55">
         <v>0.01</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B51">
+      <c r="B56">
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52">
+      <c r="B57">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B58" t="s">
         <v>65</v>
       </c>
-      <c r="B53" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59">
+        <v>0.05</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60">
+        <v>2.5</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B54">
-        <v>0.05</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55">
+      <c r="B61">
+        <v>6.7</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62">
+        <v>6.8</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63">
+        <v>1.29</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64">
+        <v>3.85</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65">
+        <v>3.73</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67">
+        <v>0.184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="3">
+        <v>6.2E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71">
+        <v>0.67</v>
+      </c>
+      <c r="D71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81">
+        <v>0.06</v>
+      </c>
+      <c r="D81" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87">
+        <v>1.08</v>
+      </c>
+      <c r="D87" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>71</v>
+      </c>
+      <c r="B88">
         <v>2.5</v>
       </c>
-      <c r="G55" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56">
-        <v>6.7</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57">
-        <v>6.8</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58">
-        <v>1.29</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-      <c r="C59">
-        <v>3.85</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60">
-        <v>3.73</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B61">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62">
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B63">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="3">
-        <v>6.2E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B65">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>73</v>
-      </c>
-      <c r="B66">
-        <v>0.67</v>
-      </c>
-      <c r="D66" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>74</v>
-      </c>
-      <c r="B67">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>75</v>
-      </c>
-      <c r="B68">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>76</v>
-      </c>
-      <c r="B69">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>77</v>
-      </c>
-      <c r="B70">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>78</v>
-      </c>
-      <c r="B71">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>82</v>
-      </c>
-      <c r="B72">
-        <v>2.36</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>79</v>
-      </c>
-      <c r="B73">
-        <v>2.21</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>80</v>
-      </c>
-      <c r="B74">
-        <v>4.3600000000000003</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>81</v>
-      </c>
-      <c r="B75">
-        <v>1.48</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>83</v>
-      </c>
-      <c r="B76">
-        <v>0.06</v>
-      </c>
-      <c r="D76" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>84</v>
-      </c>
-      <c r="B77">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>85</v>
-      </c>
-      <c r="B78">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>86</v>
-      </c>
-      <c r="B79">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>87</v>
-      </c>
-      <c r="B80">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>88</v>
-      </c>
-      <c r="B81">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B82">
-        <v>1.08</v>
-      </c>
-      <c r="D82" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>72</v>
-      </c>
-      <c r="B83">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B84">
+      <c r="B89">
         <v>0.7</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B85">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B86">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B87">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B88">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B89">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="B90">
         <v>0.7</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>138</v>
+        <v>33</v>
       </c>
       <c r="B91">
         <v>0.7</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B93">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B95">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B96">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B97">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B92">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B93">
+      <c r="B98">
         <v>0.7</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>61</v>
-      </c>
-      <c r="B94">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>60</v>
+      </c>
+      <c r="B99">
         <v>0.7</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B95">
-        <v>0.4</v>
-      </c>
-      <c r="C95" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B96">
-        <v>0.8</v>
-      </c>
-      <c r="C96" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B97">
-        <v>0.9</v>
-      </c>
-      <c r="C97" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B98">
-        <v>0.25</v>
-      </c>
-      <c r="C98" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B99">
-        <v>0.5</v>
-      </c>
-      <c r="C99" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="B100">
         <v>0.8</v>
       </c>
       <c r="C100" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B101">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="C101" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B102">
         <v>0.25</v>
       </c>
       <c r="C102" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B103">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="C103" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B104">
         <v>0.8</v>
       </c>
       <c r="C104" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B105">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="C105" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B106">
+        <v>0.25</v>
+      </c>
+      <c r="C106" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B106">
-        <v>0.6</v>
-      </c>
-      <c r="C106" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="B107">
         <v>0.4</v>
       </c>
       <c r="C107" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B108">
         <v>0.8</v>
       </c>
       <c r="C108" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B109">
+        <v>0.3</v>
+      </c>
+      <c r="C109" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B110">
+        <v>0.6</v>
+      </c>
+      <c r="C110" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B111">
+        <v>0.4</v>
+      </c>
+      <c r="C111" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B112">
+        <v>0.8</v>
+      </c>
+      <c r="C112" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B113">
+        <v>0.5</v>
+      </c>
+      <c r="C113" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B109">
+      <c r="B114">
+        <v>0.8</v>
+      </c>
+      <c r="C114" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B115">
+        <v>0.75</v>
+      </c>
+      <c r="C115" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B116">
         <v>0.5</v>
       </c>
-      <c r="C109" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B110">
+      <c r="C116" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B117">
+        <v>0.75</v>
+      </c>
+      <c r="C117" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B118">
+        <v>0.5</v>
+      </c>
+      <c r="C118" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B119">
+        <v>0.75</v>
+      </c>
+      <c r="C119" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B120">
+        <v>0.5</v>
+      </c>
+      <c r="C120" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B121">
+        <v>0.5</v>
+      </c>
+      <c r="C121" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B122">
+        <v>0.5</v>
+      </c>
+      <c r="C122" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B123">
+        <v>0.5</v>
+      </c>
+      <c r="C123" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B124">
+        <v>0.5</v>
+      </c>
+      <c r="C124" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B125">
         <v>0.8</v>
       </c>
-      <c r="C110" t="s">
-        <v>40</v>
+      <c r="C125" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B126">
+        <v>0.5</v>
+      </c>
+      <c r="C126" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B127">
+        <v>0.75</v>
+      </c>
+      <c r="C127" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B128">
+        <v>0.5</v>
+      </c>
+      <c r="C128" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B129">
+        <v>0.8</v>
+      </c>
+      <c r="C129" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B130">
+        <v>0.5</v>
+      </c>
+      <c r="C130" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B131">
+        <v>0.5</v>
+      </c>
+      <c r="C131" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing and addition of buffer of 1 month before new pregnancy in contraception
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -1375,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,6 +1500,9 @@
         <v>2</v>
       </c>
       <c r="B11">
+        <v>0.2</v>
+      </c>
+      <c r="C11">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D11" s="2"/>
@@ -1671,6 +1674,9 @@
         <v>6</v>
       </c>
       <c r="B25">
+        <v>0.2</v>
+      </c>
+      <c r="C25">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D25" s="2"/>
@@ -1695,6 +1701,9 @@
         <v>125</v>
       </c>
       <c r="B27">
+        <v>0.2</v>
+      </c>
+      <c r="C27">
         <v>0.01</v>
       </c>
       <c r="D27" s="2"/>
@@ -1755,6 +1764,9 @@
         <v>5</v>
       </c>
       <c r="B32">
+        <v>0.2</v>
+      </c>
+      <c r="C32">
         <v>1.2E-2</v>
       </c>
       <c r="D32" s="2"/>
@@ -1767,12 +1779,14 @@
         <v>130</v>
       </c>
       <c r="B33">
+        <v>0.2</v>
+      </c>
+      <c r="C33">
         <v>0.01</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>1E-3</v>
       </c>
-      <c r="D33" s="2"/>
       <c r="G33" s="2" t="s">
         <v>134</v>
       </c>
@@ -1839,6 +1853,9 @@
         <v>9</v>
       </c>
       <c r="B39">
+        <v>0.2</v>
+      </c>
+      <c r="C39">
         <v>0.02</v>
       </c>
     </row>
@@ -1847,6 +1864,9 @@
         <v>136</v>
       </c>
       <c r="B40">
+        <v>0.2</v>
+      </c>
+      <c r="C40">
         <v>0.184</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -1858,6 +1878,9 @@
         <v>10</v>
       </c>
       <c r="B41">
+        <v>0.2</v>
+      </c>
+      <c r="C41">
         <v>0.184</v>
       </c>
     </row>
@@ -1866,6 +1889,9 @@
         <v>23</v>
       </c>
       <c r="B42">
+        <v>0.2</v>
+      </c>
+      <c r="C42">
         <v>0.33</v>
       </c>
     </row>
@@ -1874,6 +1900,9 @@
         <v>11</v>
       </c>
       <c r="B43">
+        <v>0.2</v>
+      </c>
+      <c r="C43">
         <v>0.34499999999999997</v>
       </c>
     </row>
@@ -1970,6 +1999,9 @@
         <v>14</v>
       </c>
       <c r="B55">
+        <v>0.2</v>
+      </c>
+      <c r="C55">
         <v>0.01</v>
       </c>
     </row>
@@ -1978,6 +2010,9 @@
         <v>15</v>
       </c>
       <c r="B56">
+        <v>0.2</v>
+      </c>
+      <c r="C56">
         <v>0.03</v>
       </c>
     </row>
@@ -2002,6 +2037,9 @@
         <v>117</v>
       </c>
       <c r="B59">
+        <v>0.2</v>
+      </c>
+      <c r="C59">
         <v>0.05</v>
       </c>
       <c r="G59" s="2" t="s">
@@ -2079,6 +2117,9 @@
         <v>37</v>
       </c>
       <c r="B66">
+        <v>0.2</v>
+      </c>
+      <c r="C66">
         <v>0.1</v>
       </c>
     </row>
@@ -2087,6 +2128,9 @@
         <v>17</v>
       </c>
       <c r="B67">
+        <v>0.2</v>
+      </c>
+      <c r="C67">
         <v>0.184</v>
       </c>
     </row>
@@ -2095,6 +2139,9 @@
         <v>18</v>
       </c>
       <c r="B68">
+        <v>0.2</v>
+      </c>
+      <c r="C68">
         <v>0.33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moving HSI functions out to the module
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="161">
   <si>
     <t>parameter_name</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>rr_still_birth_ur_maternal_death</t>
+  </si>
+  <si>
+    <t>prob_cure_uterotonics</t>
   </si>
 </sst>
 </file>
@@ -1373,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G131"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2364,15 +2367,15 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>68</v>
+        <v>160</v>
       </c>
       <c r="B95">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>137</v>
+        <v>68</v>
       </c>
       <c r="B96">
         <v>0.7</v>
@@ -2380,45 +2383,42 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>66</v>
+        <v>137</v>
       </c>
       <c r="B97">
-        <v>0.75</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B98">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B98">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>60</v>
       </c>
       <c r="B99">
         <v>0.7</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>38</v>
+      <c r="A100" t="s">
+        <v>60</v>
       </c>
       <c r="B100">
-        <v>0.8</v>
-      </c>
-      <c r="C100" t="s">
-        <v>39</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B101">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="C101" t="s">
         <v>39</v>
@@ -2426,27 +2426,24 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B102">
-        <v>0.4</v>
-      </c>
-      <c r="C102">
-        <v>0.25</v>
-      </c>
-      <c r="D102" t="s">
+        <v>0.9</v>
+      </c>
+      <c r="C102" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B103">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="C103">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D103" t="s">
         <v>39</v>
@@ -2454,13 +2451,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B104">
         <v>0.8</v>
       </c>
       <c r="C104">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D104" t="s">
         <v>39</v>
@@ -2468,13 +2465,13 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B105">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="C105">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="D105" t="s">
         <v>39</v>
@@ -2482,13 +2479,13 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B106">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="C106">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D106" t="s">
         <v>39</v>
@@ -2496,13 +2493,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B107">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="C107">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D107" t="s">
         <v>39</v>
@@ -2510,13 +2507,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B108">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="C108">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D108" t="s">
         <v>39</v>
@@ -2524,13 +2521,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B109">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="C109">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="D109" t="s">
         <v>39</v>
@@ -2538,13 +2535,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B110">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="C110">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="D110" t="s">
         <v>39</v>
@@ -2552,13 +2549,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B111">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="C111">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D111" t="s">
         <v>39</v>
@@ -2566,13 +2563,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B112">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="C112">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D112" t="s">
         <v>39</v>
@@ -2580,13 +2577,13 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B113">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="C113">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D113" t="s">
         <v>39</v>
@@ -2594,13 +2591,13 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B114">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="C114">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D114" t="s">
         <v>39</v>
@@ -2608,21 +2605,24 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>138</v>
+        <v>56</v>
       </c>
       <c r="B115">
-        <v>0.75</v>
-      </c>
-      <c r="C115" t="s">
+        <v>0.8</v>
+      </c>
+      <c r="C115">
+        <v>0.8</v>
+      </c>
+      <c r="D115" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B116">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C116" t="s">
         <v>39</v>
@@ -2630,10 +2630,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B117">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="C117" t="s">
         <v>39</v>
@@ -2641,10 +2641,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B118">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C118" t="s">
         <v>39</v>
@@ -2652,10 +2652,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B119">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="C119" t="s">
         <v>39</v>
@@ -2663,18 +2663,18 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B120">
+        <v>0.75</v>
+      </c>
+      <c r="C120" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B120">
-        <v>0.5</v>
-      </c>
-      <c r="C120" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="B121">
         <v>0.5</v>
@@ -2684,8 +2684,8 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>146</v>
+      <c r="A122" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="B122">
         <v>0.5</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B123">
         <v>0.5</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B124">
         <v>0.5</v>
@@ -2718,10 +2718,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B125">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="C125" t="s">
         <v>39</v>
@@ -2729,10 +2729,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B126">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C126" t="s">
         <v>39</v>
@@ -2740,10 +2740,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B127">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="C127" t="s">
         <v>39</v>
@@ -2751,10 +2751,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B128">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C128" t="s">
         <v>39</v>
@@ -2762,10 +2762,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B129">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="C129" t="s">
         <v>39</v>
@@ -2773,10 +2773,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B130">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C130" t="s">
         <v>39</v>
@@ -2784,12 +2784,23 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B131">
         <v>0.5</v>
       </c>
       <c r="C131" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B132">
+        <v>0.5</v>
+      </c>
+      <c r="C132" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
use of HSI generic appts
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -1399,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new scenario analysis, changes to death equations
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="178">
   <si>
     <t>parameter_name</t>
   </si>
@@ -558,6 +558,36 @@
   </si>
   <si>
     <t>lower_limit_postterm_days</t>
+  </si>
+  <si>
+    <t>aph_prompt_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>aph_delayed_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>ur_prompt_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>ur_delayed_treatment_effect_md</t>
+  </si>
+  <si>
+    <t>eclampsia_prompt_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>eclampsia_delayed_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>aph_prompt_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>aph_delayed_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>ur_prompt_treatment_effect_sb</t>
+  </si>
+  <si>
+    <t>ur_delayed_treatment_effect_sb</t>
   </si>
 </sst>
 </file>
@@ -1397,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2791,32 +2821,26 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="B131">
         <v>0.5</v>
       </c>
-      <c r="C131" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="B132">
-        <v>0.5</v>
-      </c>
-      <c r="C132" t="s">
-        <v>39</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B133">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="C133" t="s">
         <v>39</v>
@@ -2824,7 +2848,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B134">
         <v>0.5</v>
@@ -2835,29 +2859,23 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B135">
-        <v>0.75</v>
-      </c>
-      <c r="C135" t="s">
-        <v>39</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="B136">
-        <v>0.5</v>
-      </c>
-      <c r="C136" t="s">
-        <v>39</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B137">
         <v>0.8</v>
@@ -2868,24 +2886,122 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="B138">
         <v>0.5</v>
       </c>
-      <c r="C138" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B139">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B140">
+        <v>0.5</v>
+      </c>
+      <c r="C140" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B141">
+        <v>0.75</v>
+      </c>
+      <c r="C141" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B142">
+        <v>0.5</v>
+      </c>
+      <c r="C142" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B143">
+        <v>0.8</v>
+      </c>
+      <c r="C143" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B144">
+        <v>0.5</v>
+      </c>
+      <c r="C144" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B145">
+        <v>0.5</v>
+      </c>
+      <c r="C145" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B146">
+        <v>0.75</v>
+      </c>
+      <c r="C146" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B139">
+      <c r="B147">
         <v>0.5</v>
       </c>
-      <c r="C139" t="s">
-        <v>39</v>
+      <c r="C147" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B148">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B149">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed values in resource file from debugging values
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
+++ b/resources/ResourceFile_LabourSkilledBirthAttendance.xlsx
@@ -1409,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73:B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,9 +1597,6 @@
         <v>2</v>
       </c>
       <c r="B18">
-        <v>0.2</v>
-      </c>
-      <c r="C18">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D18" s="2"/>
@@ -1771,9 +1768,6 @@
         <v>6</v>
       </c>
       <c r="B32">
-        <v>0.2</v>
-      </c>
-      <c r="C32">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D32" s="2"/>
@@ -1785,9 +1779,6 @@
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B33">
-        <v>3.4</v>
-      </c>
       <c r="D33" s="2"/>
       <c r="G33" s="2" t="s">
         <v>31</v>
@@ -1798,9 +1789,6 @@
         <v>122</v>
       </c>
       <c r="B34">
-        <v>0.2</v>
-      </c>
-      <c r="C34">
         <v>0.01</v>
       </c>
       <c r="D34" s="2"/>
@@ -1861,9 +1849,6 @@
         <v>5</v>
       </c>
       <c r="B39">
-        <v>0.2</v>
-      </c>
-      <c r="C39">
         <v>1.2E-2</v>
       </c>
       <c r="D39" s="2"/>
@@ -1876,9 +1861,6 @@
         <v>127</v>
       </c>
       <c r="B40">
-        <v>0.2</v>
-      </c>
-      <c r="C40">
         <v>0.01</v>
       </c>
       <c r="D40">
@@ -1950,9 +1932,6 @@
         <v>9</v>
       </c>
       <c r="B46">
-        <v>0.2</v>
-      </c>
-      <c r="C46">
         <v>0.02</v>
       </c>
     </row>
@@ -1961,9 +1940,6 @@
         <v>133</v>
       </c>
       <c r="B47">
-        <v>0.2</v>
-      </c>
-      <c r="C47">
         <v>0.184</v>
       </c>
       <c r="G47" s="4" t="s">
@@ -1975,35 +1951,26 @@
         <v>10</v>
       </c>
       <c r="B48">
-        <v>0.2</v>
-      </c>
-      <c r="C48">
         <v>0.184</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B49">
-        <v>0.2</v>
-      </c>
-      <c r="C49">
         <v>0.33</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B50">
-        <v>0.2</v>
-      </c>
-      <c r="C50">
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>34</v>
       </c>
@@ -2011,7 +1978,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>137</v>
       </c>
@@ -2019,7 +1986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
@@ -2027,7 +1994,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>148</v>
       </c>
@@ -2035,7 +2002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>12</v>
       </c>
@@ -2043,7 +2010,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>144</v>
       </c>
@@ -2051,7 +2018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>35</v>
       </c>
@@ -2059,7 +2026,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>152</v>
       </c>
@@ -2067,7 +2034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>132</v>
       </c>
@@ -2075,7 +2042,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>13</v>
       </c>
@@ -2083,7 +2050,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>145</v>
       </c>
@@ -2091,29 +2058,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B62">
-        <v>0.2</v>
-      </c>
-      <c r="C62">
         <v>0.01</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B63">
-        <v>0.2</v>
-      </c>
-      <c r="C63">
         <v>0.03</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>16</v>
       </c>
@@ -2134,9 +2095,6 @@
         <v>114</v>
       </c>
       <c r="B66">
-        <v>0.2</v>
-      </c>
-      <c r="C66">
         <v>0.05</v>
       </c>
       <c r="G66" s="2" t="s">
@@ -2214,9 +2172,6 @@
         <v>36</v>
       </c>
       <c r="B73">
-        <v>0.2</v>
-      </c>
-      <c r="C73">
         <v>0.1</v>
       </c>
     </row>
@@ -2225,9 +2180,6 @@
         <v>17</v>
       </c>
       <c r="B74">
-        <v>0.2</v>
-      </c>
-      <c r="C74">
         <v>0.184</v>
       </c>
     </row>
@@ -2236,9 +2188,6 @@
         <v>18</v>
       </c>
       <c r="B75">
-        <v>0.2</v>
-      </c>
-      <c r="C75">
         <v>0.33</v>
       </c>
     </row>

</xml_diff>